<commit_message>
Adjustments to carbon tax files to account for ETS1 vs ETS2 price projection differences, free allowances, and CBAM leakage prevention
(cherry picked from commit 1cef641abd51282859517838e61817732bb92d6f)
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_TEP/fuels/BCTR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C28A361-BC9D-4B04-9AEE-B7A96C556F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6500BCC-809B-4E81-8AF7-2880CEA1FD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="1080" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="29970" yWindow="1440" windowWidth="27045" windowHeight="14490" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -370,9 +370,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -410,7 +410,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -516,7 +516,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -658,7 +658,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,18 +672,18 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -691,52 +691,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -750,7 +750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -768,7 +768,7 @@
         <v>1.3919999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -789,7 +789,7 @@
         <v>1.2847999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G20">
         <v>2013</v>
       </c>
@@ -804,7 +804,7 @@
         <v>1.3281000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G21">
         <v>2014</v>
       </c>
@@ -819,7 +819,7 @@
         <v>1.3285</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G22">
         <v>2015</v>
       </c>
@@ -834,7 +834,7 @@
         <v>1.1094999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G23">
         <v>2016</v>
       </c>
@@ -849,7 +849,7 @@
         <v>1.1069</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G24">
         <v>2017</v>
       </c>
@@ -864,7 +864,7 @@
         <v>1.1296999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G25">
         <v>2018</v>
       </c>
@@ -879,7 +879,7 @@
         <v>1.181</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G26">
         <v>2019</v>
       </c>
@@ -894,7 +894,7 @@
         <v>1.1194999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G27">
         <v>2020</v>
       </c>
@@ -905,7 +905,7 @@
         <v>1.1422000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G28">
         <v>2021</v>
       </c>
@@ -916,7 +916,7 @@
         <v>1.1827000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G29">
         <v>2022</v>
       </c>
@@ -941,9 +941,9 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -974,7 +974,7 @@
       </c>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -998,7 +998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>22</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="C11">
         <f>D11</f>
         <v>35</v>
@@ -1385,15 +1385,15 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1488,102 +1488,132 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="24">
-        <v>0</v>
+        <f t="shared" ref="B2" si="0">B3</f>
+        <v>41.540313365930324</v>
       </c>
       <c r="C2" s="24">
-        <v>0</v>
+        <f>C3</f>
+        <v>41.540313365930324</v>
       </c>
       <c r="D2" s="24">
-        <v>0</v>
+        <f t="shared" ref="D2:AE2" si="1">D3</f>
+        <v>41.540313365930324</v>
       </c>
       <c r="E2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>41.540313365930324</v>
       </c>
       <c r="F2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>41.540313365930324</v>
       </c>
       <c r="G2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>45.100911654438633</v>
       </c>
       <c r="H2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>48.66150994294695</v>
       </c>
       <c r="I2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>52.222108231455259</v>
       </c>
       <c r="J2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>55.782706519963583</v>
       </c>
       <c r="K2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>59.343304808471892</v>
       </c>
       <c r="L2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>61.717037000810762</v>
       </c>
       <c r="M2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>64.09076919314964</v>
       </c>
       <c r="N2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>66.464501385488518</v>
       </c>
       <c r="O2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>68.838233577827395</v>
       </c>
       <c r="P2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>71.211965770166259</v>
       </c>
       <c r="Q2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>73.585697962505151</v>
       </c>
       <c r="R2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>75.959430154844014</v>
       </c>
       <c r="S2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>78.333162347182892</v>
       </c>
       <c r="T2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>80.70689453952177</v>
       </c>
       <c r="U2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>83.080626731860647</v>
       </c>
       <c r="V2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>85.454358924199525</v>
       </c>
       <c r="W2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>87.828091116538388</v>
       </c>
       <c r="X2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>90.201823308877266</v>
       </c>
       <c r="Y2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>92.575555501216144</v>
       </c>
       <c r="Z2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>94.949287693555036</v>
       </c>
       <c r="AA2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>97.323019885893899</v>
       </c>
       <c r="AB2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>99.696752078232777</v>
       </c>
       <c r="AC2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>102.07048427057165</v>
       </c>
       <c r="AD2" s="24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>104.44421646291052</v>
       </c>
       <c r="AE2" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>106.8179486552494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1708,7 +1738,7 @@
         <v>106.8179486552494</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1803,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1898,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1907,123 +1937,123 @@
         <v>41.540313365930324</v>
       </c>
       <c r="C6" s="24">
-        <f t="shared" ref="C6:AE6" si="0">C3</f>
+        <f t="shared" ref="C6:AE6" si="2">C3</f>
         <v>41.540313365930324</v>
       </c>
       <c r="D6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.540313365930324</v>
       </c>
       <c r="E6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.540313365930324</v>
       </c>
       <c r="F6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.540313365930324</v>
       </c>
       <c r="G6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>45.100911654438633</v>
       </c>
       <c r="H6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>48.66150994294695</v>
       </c>
       <c r="I6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52.222108231455259</v>
       </c>
       <c r="J6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>55.782706519963583</v>
       </c>
       <c r="K6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>59.343304808471892</v>
       </c>
       <c r="L6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>61.717037000810762</v>
       </c>
       <c r="M6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64.09076919314964</v>
       </c>
       <c r="N6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>66.464501385488518</v>
       </c>
       <c r="O6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>68.838233577827395</v>
       </c>
       <c r="P6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>71.211965770166259</v>
       </c>
       <c r="Q6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>73.585697962505151</v>
       </c>
       <c r="R6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>75.959430154844014</v>
       </c>
       <c r="S6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>78.333162347182892</v>
       </c>
       <c r="T6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>80.70689453952177</v>
       </c>
       <c r="U6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>83.080626731860647</v>
       </c>
       <c r="V6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>85.454358924199525</v>
       </c>
       <c r="W6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>87.828091116538388</v>
       </c>
       <c r="X6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>90.201823308877266</v>
       </c>
       <c r="Y6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>92.575555501216144</v>
       </c>
       <c r="Z6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>94.949287693555036</v>
       </c>
       <c r="AA6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>97.323019885893899</v>
       </c>
       <c r="AB6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>99.696752078232777</v>
       </c>
       <c r="AC6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>102.07048427057165</v>
       </c>
       <c r="AD6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>104.44421646291052</v>
       </c>
       <c r="AE6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>106.8179486552494</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2118,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2315,12 +2345,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2553,29 +2585,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3810981-6F61-4C76-A985-60AA740A519D}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2584,4 +2602,31 @@
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3810981-6F61-4C76-A985-60AA740A519D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add district heat / hydrogen carbon tax
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6500BCC-809B-4E81-8AF7-2880CEA1FD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF70482E-8A53-4DE8-AD6D-A1C0AA40FB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1440" windowWidth="27045" windowHeight="14490" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="62220" yWindow="7155" windowWidth="23790" windowHeight="9675" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="calc" sheetId="3" r:id="rId2"/>
     <sheet name="BCTR" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1385,7 +1385,7 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE2"/>
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2058,94 +2058,124 @@
         <v>9</v>
       </c>
       <c r="B7" s="24">
-        <v>0</v>
+        <f>B6*0.75*0.6</f>
+        <v>18.693141014668644</v>
       </c>
       <c r="C7" s="24">
-        <v>0</v>
+        <f t="shared" ref="C7:AE7" si="3">C6*0.75*0.6</f>
+        <v>18.693141014668644</v>
       </c>
       <c r="D7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>18.693141014668644</v>
       </c>
       <c r="E7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>18.693141014668644</v>
       </c>
       <c r="F7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>18.693141014668644</v>
       </c>
       <c r="G7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>20.295410244497386</v>
       </c>
       <c r="H7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>21.897679474326125</v>
       </c>
       <c r="I7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>23.499948704154868</v>
       </c>
       <c r="J7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>25.10221793398361</v>
       </c>
       <c r="K7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>26.704487163812352</v>
       </c>
       <c r="L7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>27.772666650364844</v>
       </c>
       <c r="M7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>28.840846136917335</v>
       </c>
       <c r="N7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>29.90902562346983</v>
       </c>
       <c r="O7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>30.977205110022325</v>
       </c>
       <c r="P7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>32.045384596574813</v>
       </c>
       <c r="Q7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>33.113564083127315</v>
       </c>
       <c r="R7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>34.181743569679803</v>
       </c>
       <c r="S7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>35.249923056232298</v>
       </c>
       <c r="T7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>36.318102542784793</v>
       </c>
       <c r="U7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>37.386282029337288</v>
       </c>
       <c r="V7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>38.454461515889783</v>
       </c>
       <c r="W7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>39.522641002442271</v>
       </c>
       <c r="X7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>40.590820488994773</v>
       </c>
       <c r="Y7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>41.65899997554726</v>
       </c>
       <c r="Z7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>42.727179462099762</v>
       </c>
       <c r="AA7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>43.79535894865225</v>
       </c>
       <c r="AB7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>44.863538435204752</v>
       </c>
       <c r="AC7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>45.93171792175724</v>
       </c>
       <c r="AD7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>46.999897408309735</v>
       </c>
       <c r="AE7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>48.06807689486223</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Align BCTR currency conversion with EPS convention
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF70482E-8A53-4DE8-AD6D-A1C0AA40FB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4948291-3129-4D25-A452-09947A65D3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62220" yWindow="7155" windowWidth="23790" windowHeight="9675" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="10200" yWindow="3405" windowWidth="18555" windowHeight="9120" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>BCTR BAU Carbon Tax Rate</t>
   </si>
@@ -106,12 +106,6 @@
     <t>CO2 price [€/t]</t>
   </si>
   <si>
-    <t>inflation correction</t>
-  </si>
-  <si>
-    <t>exchange rate 2012</t>
-  </si>
-  <si>
     <t>inflation rate EU27_2020</t>
   </si>
   <si>
@@ -146,6 +140,18 @@
   </si>
   <si>
     <t>90 in 2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation correction    1 USD 2019 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange rate     1 EUR 2019 = </t>
+  </si>
+  <si>
+    <t>USD 2012</t>
+  </si>
+  <si>
+    <t>USD 2019</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -295,11 +301,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,6 +367,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,14 +687,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -693,42 +714,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -738,25 +759,28 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <f>1/I26</f>
-        <v>0.9237749814519286</v>
+      <c r="B18" s="26">
+        <f>1/1.1135</f>
+        <v>0.89806915132465204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2011</v>
@@ -769,12 +793,15 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
+      <c r="A19" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="22">
-        <f>J19</f>
-        <v>1.2847999999999999</v>
+        <f>J26</f>
+        <v>1.1198999999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
       </c>
       <c r="G19">
         <v>2012</v>
@@ -891,7 +918,7 @@
         <v>1.0825147033407052</v>
       </c>
       <c r="J26" s="22">
-        <v>1.1194999999999999</v>
+        <v>1.1198999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -938,7 +965,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -1385,7 +1412,7 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AE7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,123 +1521,123 @@
       </c>
       <c r="B2" s="24">
         <f t="shared" ref="B2" si="0">B3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C2" s="24">
         <f>C3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D2" s="24">
         <f t="shared" ref="D2:AE2" si="1">D3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E2" s="24">
         <f t="shared" si="1"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F2" s="24">
         <f t="shared" si="1"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G2" s="24">
         <f t="shared" si="1"/>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H2" s="24">
         <f t="shared" si="1"/>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I2" s="24">
         <f t="shared" si="1"/>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J2" s="24">
         <f t="shared" si="1"/>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K2" s="24">
         <f t="shared" si="1"/>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L2" s="24">
         <f t="shared" si="1"/>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M2" s="24">
         <f t="shared" si="1"/>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N2" s="24">
         <f t="shared" si="1"/>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O2" s="24">
         <f t="shared" si="1"/>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P2" s="24">
         <f t="shared" si="1"/>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q2" s="24">
         <f t="shared" si="1"/>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R2" s="24">
         <f t="shared" si="1"/>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S2" s="24">
         <f t="shared" si="1"/>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T2" s="24">
         <f t="shared" si="1"/>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U2" s="24">
         <f t="shared" si="1"/>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V2" s="24">
         <f t="shared" si="1"/>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W2" s="24">
         <f t="shared" si="1"/>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X2" s="24">
         <f t="shared" si="1"/>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y2" s="24">
         <f t="shared" si="1"/>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z2" s="24">
         <f t="shared" si="1"/>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA2" s="24">
         <f t="shared" si="1"/>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB2" s="24">
         <f t="shared" si="1"/>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC2" s="24">
         <f t="shared" si="1"/>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD2" s="24">
         <f t="shared" si="1"/>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE2" s="24">
         <f t="shared" si="1"/>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -1619,123 +1646,123 @@
       </c>
       <c r="B3" s="24">
         <f>calc!C11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C3" s="24">
         <f>calc!D11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D3" s="24">
         <f>calc!E11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E3" s="24">
         <f>calc!F11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F3" s="24">
         <f>calc!G11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G3" s="24">
         <f>calc!H11*About!$B$18*About!$B$19</f>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H3" s="24">
         <f>calc!I11*About!$B$18*About!$B$19</f>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I3" s="24">
         <f>calc!J11*About!$B$18*About!$B$19</f>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J3" s="24">
         <f>calc!K11*About!$B$18*About!$B$19</f>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K3" s="24">
         <f>calc!L11*About!$B$18*About!$B$19</f>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L3" s="24">
         <f>calc!M11*About!$B$18*About!$B$19</f>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M3" s="24">
         <f>calc!N11*About!$B$18*About!$B$19</f>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N3" s="24">
         <f>calc!O11*About!$B$18*About!$B$19</f>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O3" s="24">
         <f>calc!P11*About!$B$18*About!$B$19</f>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P3" s="24">
         <f>calc!Q11*About!$B$18*About!$B$19</f>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q3" s="24">
         <f>calc!R11*About!$B$18*About!$B$19</f>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R3" s="24">
         <f>calc!S11*About!$B$18*About!$B$19</f>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S3" s="24">
         <f>calc!T11*About!$B$18*About!$B$19</f>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T3" s="24">
         <f>calc!U11*About!$B$18*About!$B$19</f>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U3" s="24">
         <f>calc!V11*About!$B$18*About!$B$19</f>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V3" s="24">
         <f>calc!W11*About!$B$18*About!$B$19</f>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W3" s="24">
         <f>calc!X11*About!$B$18*About!$B$19</f>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X3" s="24">
         <f>calc!Y11*About!$B$18*About!$B$19</f>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y3" s="24">
         <f>calc!Z11*About!$B$18*About!$B$19</f>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z3" s="24">
         <f>calc!AA11*About!$B$18*About!$B$19</f>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA3" s="24">
         <f>calc!AB11*About!$B$18*About!$B$19</f>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB3" s="24">
         <f>calc!AC11*About!$B$18*About!$B$19</f>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC3" s="24">
         <f>calc!AD11*About!$B$18*About!$B$19</f>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD3" s="24">
         <f>calc!AE11*About!$B$18*About!$B$19</f>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE3" s="24">
         <f>calc!AF11*About!$B$18*About!$B$19</f>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -1934,123 +1961,123 @@
       </c>
       <c r="B6" s="24">
         <f>B3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C6" s="24">
         <f t="shared" ref="C6:AE6" si="2">C3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G6" s="24">
         <f t="shared" si="2"/>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H6" s="24">
         <f t="shared" si="2"/>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I6" s="24">
         <f t="shared" si="2"/>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J6" s="24">
         <f t="shared" si="2"/>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K6" s="24">
         <f t="shared" si="2"/>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L6" s="24">
         <f t="shared" si="2"/>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M6" s="24">
         <f t="shared" si="2"/>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N6" s="24">
         <f t="shared" si="2"/>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O6" s="24">
         <f t="shared" si="2"/>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P6" s="24">
         <f t="shared" si="2"/>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q6" s="24">
         <f t="shared" si="2"/>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R6" s="24">
         <f t="shared" si="2"/>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S6" s="24">
         <f t="shared" si="2"/>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T6" s="24">
         <f t="shared" si="2"/>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U6" s="24">
         <f t="shared" si="2"/>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V6" s="24">
         <f t="shared" si="2"/>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W6" s="24">
         <f t="shared" si="2"/>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X6" s="24">
         <f t="shared" si="2"/>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y6" s="24">
         <f t="shared" si="2"/>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z6" s="24">
         <f t="shared" si="2"/>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA6" s="24">
         <f t="shared" si="2"/>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB6" s="24">
         <f t="shared" si="2"/>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC6" s="24">
         <f t="shared" si="2"/>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD6" s="24">
         <f t="shared" si="2"/>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE6" s="24">
         <f t="shared" si="2"/>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -2059,123 +2086,123 @@
       </c>
       <c r="B7" s="24">
         <f>B6*0.75*0.6</f>
-        <v>18.693141014668644</v>
+        <v>15.840525370453523</v>
       </c>
       <c r="C7" s="24">
         <f t="shared" ref="C7:AE7" si="3">C6*0.75*0.6</f>
-        <v>18.693141014668644</v>
+        <v>15.840525370453523</v>
       </c>
       <c r="D7" s="24">
         <f t="shared" si="3"/>
-        <v>18.693141014668644</v>
+        <v>15.840525370453523</v>
       </c>
       <c r="E7" s="24">
         <f t="shared" si="3"/>
-        <v>18.693141014668644</v>
+        <v>15.840525370453523</v>
       </c>
       <c r="F7" s="24">
         <f t="shared" si="3"/>
-        <v>18.693141014668644</v>
+        <v>15.840525370453523</v>
       </c>
       <c r="G7" s="24">
         <f t="shared" si="3"/>
-        <v>20.295410244497386</v>
+        <v>17.198284687920971</v>
       </c>
       <c r="H7" s="24">
         <f t="shared" si="3"/>
-        <v>21.897679474326125</v>
+        <v>18.556044005388411</v>
       </c>
       <c r="I7" s="24">
         <f t="shared" si="3"/>
-        <v>23.499948704154868</v>
+        <v>19.913803322855859</v>
       </c>
       <c r="J7" s="24">
         <f t="shared" si="3"/>
-        <v>25.10221793398361</v>
+        <v>21.271562640323303</v>
       </c>
       <c r="K7" s="24">
         <f t="shared" si="3"/>
-        <v>26.704487163812352</v>
+        <v>22.629321957790751</v>
       </c>
       <c r="L7" s="24">
         <f t="shared" si="3"/>
-        <v>27.772666650364844</v>
+        <v>23.534494836102382</v>
       </c>
       <c r="M7" s="24">
         <f t="shared" si="3"/>
-        <v>28.840846136917335</v>
+        <v>24.439667714414011</v>
       </c>
       <c r="N7" s="24">
         <f t="shared" si="3"/>
-        <v>29.90902562346983</v>
+        <v>25.344840592725642</v>
       </c>
       <c r="O7" s="24">
         <f t="shared" si="3"/>
-        <v>30.977205110022325</v>
+        <v>26.250013471037267</v>
       </c>
       <c r="P7" s="24">
         <f t="shared" si="3"/>
-        <v>32.045384596574813</v>
+        <v>27.155186349348895</v>
       </c>
       <c r="Q7" s="24">
         <f t="shared" si="3"/>
-        <v>33.113564083127315</v>
+        <v>28.060359227660527</v>
       </c>
       <c r="R7" s="24">
         <f t="shared" si="3"/>
-        <v>34.181743569679803</v>
+        <v>28.965532105972155</v>
       </c>
       <c r="S7" s="24">
         <f t="shared" si="3"/>
-        <v>35.249923056232298</v>
+        <v>29.870704984283787</v>
       </c>
       <c r="T7" s="24">
         <f t="shared" si="3"/>
-        <v>36.318102542784793</v>
+        <v>30.775877862595415</v>
       </c>
       <c r="U7" s="24">
         <f t="shared" si="3"/>
-        <v>37.386282029337288</v>
+        <v>31.681050740907047</v>
       </c>
       <c r="V7" s="24">
         <f t="shared" si="3"/>
-        <v>38.454461515889783</v>
+        <v>32.586223619218678</v>
       </c>
       <c r="W7" s="24">
         <f t="shared" si="3"/>
-        <v>39.522641002442271</v>
+        <v>33.49139649753031</v>
       </c>
       <c r="X7" s="24">
         <f t="shared" si="3"/>
-        <v>40.590820488994773</v>
+        <v>34.396569375841942</v>
       </c>
       <c r="Y7" s="24">
         <f t="shared" si="3"/>
-        <v>41.65899997554726</v>
+        <v>35.301742254153567</v>
       </c>
       <c r="Z7" s="24">
         <f t="shared" si="3"/>
-        <v>42.727179462099762</v>
+        <v>36.206915132465198</v>
       </c>
       <c r="AA7" s="24">
         <f t="shared" si="3"/>
-        <v>43.79535894865225</v>
+        <v>37.112088010776823</v>
       </c>
       <c r="AB7" s="24">
         <f t="shared" si="3"/>
-        <v>44.863538435204752</v>
+        <v>38.017260889088462</v>
       </c>
       <c r="AC7" s="24">
         <f t="shared" si="3"/>
-        <v>45.93171792175724</v>
+        <v>38.922433767400086</v>
       </c>
       <c r="AD7" s="24">
         <f t="shared" si="3"/>
-        <v>46.999897408309735</v>
+        <v>39.827606645711718</v>
       </c>
       <c r="AE7" s="24">
         <f t="shared" si="3"/>
-        <v>48.06807689486223</v>
+        <v>40.732779524023343</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
@@ -2375,17 +2402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -2614,6 +2630,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2624,17 +2651,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3810981-6F61-4C76-A985-60AA740A519D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2653,6 +2669,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix BCTR currency conversion (cherry picked from CI branch)
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6500BCC-809B-4E81-8AF7-2880CEA1FD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4948291-3129-4D25-A452-09947A65D3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1440" windowWidth="27045" windowHeight="14490" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="10200" yWindow="3405" windowWidth="18555" windowHeight="9120" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="calc" sheetId="3" r:id="rId2"/>
     <sheet name="BCTR" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>BCTR BAU Carbon Tax Rate</t>
   </si>
@@ -106,12 +106,6 @@
     <t>CO2 price [€/t]</t>
   </si>
   <si>
-    <t>inflation correction</t>
-  </si>
-  <si>
-    <t>exchange rate 2012</t>
-  </si>
-  <si>
     <t>inflation rate EU27_2020</t>
   </si>
   <si>
@@ -146,6 +140,18 @@
   </si>
   <si>
     <t>90 in 2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflation correction    1 USD 2019 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange rate     1 EUR 2019 = </t>
+  </si>
+  <si>
+    <t>USD 2012</t>
+  </si>
+  <si>
+    <t>USD 2019</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -295,11 +301,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,6 +367,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,14 +687,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -693,42 +714,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -738,25 +759,28 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <f>1/I26</f>
-        <v>0.9237749814519286</v>
+      <c r="B18" s="26">
+        <f>1/1.1135</f>
+        <v>0.89806915132465204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2011</v>
@@ -769,12 +793,15 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
+      <c r="A19" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="22">
-        <f>J19</f>
-        <v>1.2847999999999999</v>
+        <f>J26</f>
+        <v>1.1198999999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
       </c>
       <c r="G19">
         <v>2012</v>
@@ -891,7 +918,7 @@
         <v>1.0825147033407052</v>
       </c>
       <c r="J26" s="22">
-        <v>1.1194999999999999</v>
+        <v>1.1198999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -938,7 +965,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -1385,7 +1412,7 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,123 +1521,123 @@
       </c>
       <c r="B2" s="24">
         <f t="shared" ref="B2" si="0">B3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C2" s="24">
         <f>C3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D2" s="24">
         <f t="shared" ref="D2:AE2" si="1">D3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E2" s="24">
         <f t="shared" si="1"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F2" s="24">
         <f t="shared" si="1"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G2" s="24">
         <f t="shared" si="1"/>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H2" s="24">
         <f t="shared" si="1"/>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I2" s="24">
         <f t="shared" si="1"/>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J2" s="24">
         <f t="shared" si="1"/>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K2" s="24">
         <f t="shared" si="1"/>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L2" s="24">
         <f t="shared" si="1"/>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M2" s="24">
         <f t="shared" si="1"/>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N2" s="24">
         <f t="shared" si="1"/>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O2" s="24">
         <f t="shared" si="1"/>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P2" s="24">
         <f t="shared" si="1"/>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q2" s="24">
         <f t="shared" si="1"/>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R2" s="24">
         <f t="shared" si="1"/>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S2" s="24">
         <f t="shared" si="1"/>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T2" s="24">
         <f t="shared" si="1"/>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U2" s="24">
         <f t="shared" si="1"/>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V2" s="24">
         <f t="shared" si="1"/>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W2" s="24">
         <f t="shared" si="1"/>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X2" s="24">
         <f t="shared" si="1"/>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y2" s="24">
         <f t="shared" si="1"/>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z2" s="24">
         <f t="shared" si="1"/>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA2" s="24">
         <f t="shared" si="1"/>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB2" s="24">
         <f t="shared" si="1"/>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC2" s="24">
         <f t="shared" si="1"/>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD2" s="24">
         <f t="shared" si="1"/>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE2" s="24">
         <f t="shared" si="1"/>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -1619,123 +1646,123 @@
       </c>
       <c r="B3" s="24">
         <f>calc!C11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C3" s="24">
         <f>calc!D11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D3" s="24">
         <f>calc!E11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E3" s="24">
         <f>calc!F11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F3" s="24">
         <f>calc!G11*About!$B$18*About!$B$19</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G3" s="24">
         <f>calc!H11*About!$B$18*About!$B$19</f>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H3" s="24">
         <f>calc!I11*About!$B$18*About!$B$19</f>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I3" s="24">
         <f>calc!J11*About!$B$18*About!$B$19</f>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J3" s="24">
         <f>calc!K11*About!$B$18*About!$B$19</f>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K3" s="24">
         <f>calc!L11*About!$B$18*About!$B$19</f>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L3" s="24">
         <f>calc!M11*About!$B$18*About!$B$19</f>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M3" s="24">
         <f>calc!N11*About!$B$18*About!$B$19</f>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N3" s="24">
         <f>calc!O11*About!$B$18*About!$B$19</f>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O3" s="24">
         <f>calc!P11*About!$B$18*About!$B$19</f>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P3" s="24">
         <f>calc!Q11*About!$B$18*About!$B$19</f>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q3" s="24">
         <f>calc!R11*About!$B$18*About!$B$19</f>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R3" s="24">
         <f>calc!S11*About!$B$18*About!$B$19</f>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S3" s="24">
         <f>calc!T11*About!$B$18*About!$B$19</f>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T3" s="24">
         <f>calc!U11*About!$B$18*About!$B$19</f>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U3" s="24">
         <f>calc!V11*About!$B$18*About!$B$19</f>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V3" s="24">
         <f>calc!W11*About!$B$18*About!$B$19</f>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W3" s="24">
         <f>calc!X11*About!$B$18*About!$B$19</f>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X3" s="24">
         <f>calc!Y11*About!$B$18*About!$B$19</f>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y3" s="24">
         <f>calc!Z11*About!$B$18*About!$B$19</f>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z3" s="24">
         <f>calc!AA11*About!$B$18*About!$B$19</f>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA3" s="24">
         <f>calc!AB11*About!$B$18*About!$B$19</f>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB3" s="24">
         <f>calc!AC11*About!$B$18*About!$B$19</f>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC3" s="24">
         <f>calc!AD11*About!$B$18*About!$B$19</f>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD3" s="24">
         <f>calc!AE11*About!$B$18*About!$B$19</f>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE3" s="24">
         <f>calc!AF11*About!$B$18*About!$B$19</f>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -1934,123 +1961,123 @@
       </c>
       <c r="B6" s="24">
         <f>B3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="C6" s="24">
         <f t="shared" ref="C6:AE6" si="2">C3</f>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="D6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="E6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="F6" s="24">
         <f t="shared" si="2"/>
-        <v>41.540313365930324</v>
+        <v>35.201167489896719</v>
       </c>
       <c r="G6" s="24">
         <f t="shared" si="2"/>
-        <v>45.100911654438633</v>
+        <v>38.218410417602158</v>
       </c>
       <c r="H6" s="24">
         <f t="shared" si="2"/>
-        <v>48.66150994294695</v>
+        <v>41.235653345307583</v>
       </c>
       <c r="I6" s="24">
         <f t="shared" si="2"/>
-        <v>52.222108231455259</v>
+        <v>44.252896273013022</v>
       </c>
       <c r="J6" s="24">
         <f t="shared" si="2"/>
-        <v>55.782706519963583</v>
+        <v>47.270139200718454</v>
       </c>
       <c r="K6" s="24">
         <f t="shared" si="2"/>
-        <v>59.343304808471892</v>
+        <v>50.287382128423886</v>
       </c>
       <c r="L6" s="24">
         <f t="shared" si="2"/>
-        <v>61.717037000810762</v>
+        <v>52.298877413560845</v>
       </c>
       <c r="M6" s="24">
         <f t="shared" si="2"/>
-        <v>64.09076919314964</v>
+        <v>54.310372698697797</v>
       </c>
       <c r="N6" s="24">
         <f t="shared" si="2"/>
-        <v>66.464501385488518</v>
+        <v>56.321867983834757</v>
       </c>
       <c r="O6" s="24">
         <f t="shared" si="2"/>
-        <v>68.838233577827395</v>
+        <v>58.333363268971709</v>
       </c>
       <c r="P6" s="24">
         <f t="shared" si="2"/>
-        <v>71.211965770166259</v>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q6" s="24">
         <f t="shared" si="2"/>
-        <v>73.585697962505151</v>
+        <v>62.356353839245621</v>
       </c>
       <c r="R6" s="24">
         <f t="shared" si="2"/>
-        <v>75.959430154844014</v>
+        <v>64.367849124382573</v>
       </c>
       <c r="S6" s="24">
         <f t="shared" si="2"/>
-        <v>78.333162347182892</v>
+        <v>66.379344409519533</v>
       </c>
       <c r="T6" s="24">
         <f t="shared" si="2"/>
-        <v>80.70689453952177</v>
+        <v>68.390839694656478</v>
       </c>
       <c r="U6" s="24">
         <f t="shared" si="2"/>
-        <v>83.080626731860647</v>
+        <v>70.402334979793437</v>
       </c>
       <c r="V6" s="24">
         <f t="shared" si="2"/>
-        <v>85.454358924199525</v>
+        <v>72.413830264930397</v>
       </c>
       <c r="W6" s="24">
         <f t="shared" si="2"/>
-        <v>87.828091116538388</v>
+        <v>74.425325550067356</v>
       </c>
       <c r="X6" s="24">
         <f t="shared" si="2"/>
-        <v>90.201823308877266</v>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y6" s="24">
         <f t="shared" si="2"/>
-        <v>92.575555501216144</v>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z6" s="24">
         <f t="shared" si="2"/>
-        <v>94.949287693555036</v>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA6" s="24">
         <f t="shared" si="2"/>
-        <v>97.323019885893899</v>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB6" s="24">
         <f t="shared" si="2"/>
-        <v>99.696752078232777</v>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC6" s="24">
         <f t="shared" si="2"/>
-        <v>102.07048427057165</v>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD6" s="24">
         <f t="shared" si="2"/>
-        <v>104.44421646291052</v>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE6" s="24">
         <f t="shared" si="2"/>
-        <v>106.8179486552494</v>
+        <v>90.517287831162989</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -2058,94 +2085,124 @@
         <v>9</v>
       </c>
       <c r="B7" s="24">
-        <v>0</v>
+        <f>B6*0.75*0.6</f>
+        <v>15.840525370453523</v>
       </c>
       <c r="C7" s="24">
-        <v>0</v>
+        <f t="shared" ref="C7:AE7" si="3">C6*0.75*0.6</f>
+        <v>15.840525370453523</v>
       </c>
       <c r="D7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>15.840525370453523</v>
       </c>
       <c r="E7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>15.840525370453523</v>
       </c>
       <c r="F7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>15.840525370453523</v>
       </c>
       <c r="G7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>17.198284687920971</v>
       </c>
       <c r="H7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>18.556044005388411</v>
       </c>
       <c r="I7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>19.913803322855859</v>
       </c>
       <c r="J7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>21.271562640323303</v>
       </c>
       <c r="K7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>22.629321957790751</v>
       </c>
       <c r="L7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>23.534494836102382</v>
       </c>
       <c r="M7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>24.439667714414011</v>
       </c>
       <c r="N7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>25.344840592725642</v>
       </c>
       <c r="O7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>26.250013471037267</v>
       </c>
       <c r="P7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>27.155186349348895</v>
       </c>
       <c r="Q7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>28.060359227660527</v>
       </c>
       <c r="R7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>28.965532105972155</v>
       </c>
       <c r="S7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>29.870704984283787</v>
       </c>
       <c r="T7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>30.775877862595415</v>
       </c>
       <c r="U7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>31.681050740907047</v>
       </c>
       <c r="V7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>32.586223619218678</v>
       </c>
       <c r="W7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>33.49139649753031</v>
       </c>
       <c r="X7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>34.396569375841942</v>
       </c>
       <c r="Y7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>35.301742254153567</v>
       </c>
       <c r="Z7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>36.206915132465198</v>
       </c>
       <c r="AA7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>37.112088010776823</v>
       </c>
       <c r="AB7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>38.017260889088462</v>
       </c>
       <c r="AC7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>38.922433767400086</v>
       </c>
       <c r="AD7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>39.827606645711718</v>
       </c>
       <c r="AE7" s="24">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>40.732779524023343</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
@@ -2345,17 +2402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -2584,6 +2630,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2594,17 +2651,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3810981-6F61-4C76-A985-60AA740A519D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2623,6 +2669,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updates carbon tax projections per new Reuters analysis published 4/30/24; updates FF55.cin, FoPITY, fraction of industry/vehicle type files to match
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -1,23 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4948291-3129-4D25-A452-09947A65D3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0C3324-D266-4D73-9019-F7DAF02861D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="3405" windowWidth="18555" windowHeight="9120" activeTab="2" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="3765" yWindow="3510" windowWidth="21600" windowHeight="11235" activeTab="3" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="calc" sheetId="3" r:id="rId2"/>
-    <sheet name="BCTR" sheetId="2" r:id="rId3"/>
+    <sheet name="Allowance Schedule" sheetId="4" r:id="rId3"/>
+    <sheet name="BCTR" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="CH4_to_CO2e">'[2]Cross-Page Data'!$C$12</definedName>
+    <definedName name="cpi_2010to2012">#REF!</definedName>
+    <definedName name="cpi_2013to2012">#REF!</definedName>
+    <definedName name="cpi_2014to2012">#REF!</definedName>
+    <definedName name="cpi_2016to2012">#REF!</definedName>
+    <definedName name="gigwatts_to_megawatts">[3]About!$A$31</definedName>
+    <definedName name="N2O_to_CO2e">'[2]Cross-Page Data'!$C$13</definedName>
+    <definedName name="unit_conv">[4]About!$A$123</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>BCTR BAU Carbon Tax Rate</t>
   </si>
@@ -153,6 +170,60 @@
   <si>
     <t>USD 2019</t>
   </si>
+  <si>
+    <t>In order to help prevent industries from leaving the EU, a large share of allowances are freely granted in early years.</t>
+  </si>
+  <si>
+    <t>Share of Allowances Freely Granted</t>
+  </si>
+  <si>
+    <t>High-leak-risk industries</t>
+  </si>
+  <si>
+    <t>Other industries</t>
+  </si>
+  <si>
+    <t>Share of Allowances Auctioned</t>
+  </si>
+  <si>
+    <t>As a hydrogen production is part of a sector (industrial gases manufacturing) considered at risk of carbon leakage, installations can benefit from free allocation of ETS allowances.</t>
+  </si>
+  <si>
+    <t>https://www.europarl.europa.eu/RegData/etudes/BRIE/2023/747085/EPRS_BRI(2023)747085_EN.pdf</t>
+  </si>
+  <si>
+    <t>We use the 2022 share of emissions from H2 production as a % of H2/DH production to allocate free allowances to the H2/DH sector.</t>
+  </si>
+  <si>
+    <t>Time (Year)</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[transportation sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[electricity sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[residential buildings sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[commercial buildings sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[industry sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[district heat and hydrogen sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[LULUCF sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Total CO2e Emissions by Sector[geoengineering sector] : nosettings</t>
+  </si>
+  <si>
+    <t>Hydrogen Sector CO2e Emissions : nosettings</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +233,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +253,21 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -311,10 +397,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -371,9 +459,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -386,6 +479,1873 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Share of Allowances Auctioned</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Allowance Schedule'!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High-leak-risk industries</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Allowance Schedule'!$C$14:$AG$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Allowance Schedule'!$C$15:$AG$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5000000000000022E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0000000000000044E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.73499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4A8-406D-96B8-A3E8B88B91C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Allowance Schedule'!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Other industries</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Allowance Schedule'!$C$14:$AG$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Allowance Schedule'!$C$16:$AG$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E4A8-406D-96B8-A3E8B88B91C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1397311024"/>
+        <c:axId val="1397299984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1397311024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1397299984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1397299984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.01"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1397311024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2997200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19948E9D-61E9-4D23-99EB-1B0D08B9F8AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="Carbon Leakage Risk"/>
+      <sheetName val="Allowance Schedule"/>
+      <sheetName val="ETS Coverage"/>
+      <sheetName val="Calcs"/>
+      <sheetName val="BFoICStCT"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="9">
+          <cell r="C9">
+            <v>2020</v>
+          </cell>
+          <cell r="D9">
+            <v>2021</v>
+          </cell>
+          <cell r="E9">
+            <v>2022</v>
+          </cell>
+          <cell r="F9">
+            <v>2023</v>
+          </cell>
+          <cell r="G9">
+            <v>2024</v>
+          </cell>
+          <cell r="H9">
+            <v>2025</v>
+          </cell>
+          <cell r="I9">
+            <v>2026</v>
+          </cell>
+          <cell r="J9">
+            <v>2027</v>
+          </cell>
+          <cell r="K9">
+            <v>2028</v>
+          </cell>
+          <cell r="L9">
+            <v>2029</v>
+          </cell>
+          <cell r="M9">
+            <v>2030</v>
+          </cell>
+          <cell r="N9">
+            <v>2031</v>
+          </cell>
+          <cell r="O9">
+            <v>2032</v>
+          </cell>
+          <cell r="P9">
+            <v>2033</v>
+          </cell>
+          <cell r="Q9">
+            <v>2034</v>
+          </cell>
+          <cell r="R9">
+            <v>2035</v>
+          </cell>
+          <cell r="S9">
+            <v>2036</v>
+          </cell>
+          <cell r="T9">
+            <v>2037</v>
+          </cell>
+          <cell r="U9">
+            <v>2038</v>
+          </cell>
+          <cell r="V9">
+            <v>2039</v>
+          </cell>
+          <cell r="W9">
+            <v>2040</v>
+          </cell>
+          <cell r="X9">
+            <v>2041</v>
+          </cell>
+          <cell r="Y9">
+            <v>2042</v>
+          </cell>
+          <cell r="Z9">
+            <v>2043</v>
+          </cell>
+          <cell r="AA9">
+            <v>2044</v>
+          </cell>
+          <cell r="AB9">
+            <v>2045</v>
+          </cell>
+          <cell r="AC9">
+            <v>2046</v>
+          </cell>
+          <cell r="AD9">
+            <v>2047</v>
+          </cell>
+          <cell r="AE9">
+            <v>2048</v>
+          </cell>
+          <cell r="AF9">
+            <v>2049</v>
+          </cell>
+          <cell r="AG9">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>High-leak-risk industries</v>
+          </cell>
+          <cell r="C10">
+            <v>0</v>
+          </cell>
+          <cell r="D10">
+            <v>0</v>
+          </cell>
+          <cell r="E10">
+            <v>0</v>
+          </cell>
+          <cell r="F10">
+            <v>0</v>
+          </cell>
+          <cell r="G10">
+            <v>0</v>
+          </cell>
+          <cell r="H10">
+            <v>0</v>
+          </cell>
+          <cell r="I10">
+            <v>2.5000000000000022E-2</v>
+          </cell>
+          <cell r="J10">
+            <v>5.0000000000000044E-2</v>
+          </cell>
+          <cell r="K10">
+            <v>9.9999999999999978E-2</v>
+          </cell>
+          <cell r="L10">
+            <v>0.22499999999999998</v>
+          </cell>
+          <cell r="M10">
+            <v>0.48499999999999999</v>
+          </cell>
+          <cell r="N10">
+            <v>0.61</v>
+          </cell>
+          <cell r="O10">
+            <v>0.73499999999999999</v>
+          </cell>
+          <cell r="P10">
+            <v>0.86</v>
+          </cell>
+          <cell r="Q10">
+            <v>1</v>
+          </cell>
+          <cell r="R10">
+            <v>1</v>
+          </cell>
+          <cell r="S10">
+            <v>1</v>
+          </cell>
+          <cell r="T10">
+            <v>1</v>
+          </cell>
+          <cell r="U10">
+            <v>1</v>
+          </cell>
+          <cell r="V10">
+            <v>1</v>
+          </cell>
+          <cell r="W10">
+            <v>1</v>
+          </cell>
+          <cell r="X10">
+            <v>1</v>
+          </cell>
+          <cell r="Y10">
+            <v>1</v>
+          </cell>
+          <cell r="Z10">
+            <v>1</v>
+          </cell>
+          <cell r="AA10">
+            <v>1</v>
+          </cell>
+          <cell r="AB10">
+            <v>1</v>
+          </cell>
+          <cell r="AC10">
+            <v>1</v>
+          </cell>
+          <cell r="AD10">
+            <v>1</v>
+          </cell>
+          <cell r="AE10">
+            <v>1</v>
+          </cell>
+          <cell r="AF10">
+            <v>1</v>
+          </cell>
+          <cell r="AG10">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Other industries</v>
+          </cell>
+          <cell r="C11">
+            <v>0.7</v>
+          </cell>
+          <cell r="D11">
+            <v>0.7</v>
+          </cell>
+          <cell r="E11">
+            <v>0.7</v>
+          </cell>
+          <cell r="F11">
+            <v>0.7</v>
+          </cell>
+          <cell r="G11">
+            <v>0.7</v>
+          </cell>
+          <cell r="H11">
+            <v>0.7</v>
+          </cell>
+          <cell r="I11">
+            <v>0.7</v>
+          </cell>
+          <cell r="J11">
+            <v>0.77500000000000002</v>
+          </cell>
+          <cell r="K11">
+            <v>0.85</v>
+          </cell>
+          <cell r="L11">
+            <v>0.92500000000000004</v>
+          </cell>
+          <cell r="M11">
+            <v>1</v>
+          </cell>
+          <cell r="N11">
+            <v>1</v>
+          </cell>
+          <cell r="O11">
+            <v>1</v>
+          </cell>
+          <cell r="P11">
+            <v>1</v>
+          </cell>
+          <cell r="Q11">
+            <v>1</v>
+          </cell>
+          <cell r="R11">
+            <v>1</v>
+          </cell>
+          <cell r="S11">
+            <v>1</v>
+          </cell>
+          <cell r="T11">
+            <v>1</v>
+          </cell>
+          <cell r="U11">
+            <v>1</v>
+          </cell>
+          <cell r="V11">
+            <v>1</v>
+          </cell>
+          <cell r="W11">
+            <v>1</v>
+          </cell>
+          <cell r="X11">
+            <v>1</v>
+          </cell>
+          <cell r="Y11">
+            <v>1</v>
+          </cell>
+          <cell r="Z11">
+            <v>1</v>
+          </cell>
+          <cell r="AA11">
+            <v>1</v>
+          </cell>
+          <cell r="AB11">
+            <v>1</v>
+          </cell>
+          <cell r="AC11">
+            <v>1</v>
+          </cell>
+          <cell r="AD11">
+            <v>1</v>
+          </cell>
+          <cell r="AE11">
+            <v>1</v>
+          </cell>
+          <cell r="AF11">
+            <v>1</v>
+          </cell>
+          <cell r="AG11">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="Cross-Page Data"/>
+      <sheetName val="Non-Energy FF CO2 Emissions"/>
+      <sheetName val="Cement CO2 Emissions"/>
+      <sheetName val="Iron and Steel"/>
+      <sheetName val="Coal Mining"/>
+      <sheetName val="Natural Gas Systems"/>
+      <sheetName val="Petroleum Systems"/>
+      <sheetName val="Chem - HCFC 22 Production"/>
+      <sheetName val="Chem - ODS"/>
+      <sheetName val="Other - Aluminum"/>
+      <sheetName val="Other - Magnesium"/>
+      <sheetName val="Other - Semiconductor Mfg"/>
+      <sheetName val="Other - Elec Trans and Dist"/>
+      <sheetName val="Agriculture - EF &amp; Manure Mgmt"/>
+      <sheetName val="Agriculture - Rice Cultivation"/>
+      <sheetName val="Agriculture - Soil Mgmt"/>
+      <sheetName val="Waste - Landfills"/>
+      <sheetName val="Waste - Water Treatment"/>
+      <sheetName val="Other Industrial Processes"/>
+      <sheetName val="Combined Data"/>
+      <sheetName val="BPEiC-CO2"/>
+      <sheetName val="BPEiC-CH4"/>
+      <sheetName val="BPEiC-N2O"/>
+      <sheetName val="BPEiC-F-gases"/>
+      <sheetName val="EPA (2017) Table A3.6-1"/>
+      <sheetName val="EPA (2017) Table A3.6-7"/>
+      <sheetName val="EPA (2017) Table A3.6-10"/>
+      <sheetName val="AEO 2017_Table 6"/>
+      <sheetName val="AEO 2017_Table 11"/>
+      <sheetName val="AEO 2017_Table 13"/>
+      <sheetName val="AEO 2017_Table 15"/>
+      <sheetName val="AEO 2017_Table 19"/>
+      <sheetName val="AEO 2017_Table 20"/>
+      <sheetName val="AEO 2017_Table 24"/>
+      <sheetName val="AEO 2017_Table 62"/>
+      <sheetName val="AEO 2016_Table 6"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="12">
+          <cell r="C12">
+            <v>28</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>265</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Transport Refrigeration</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="2035 Report Deployment"/>
+      <sheetName val="2035 Report Data"/>
+      <sheetName val="EPS Output"/>
+      <sheetName val="AEO Table 9"/>
+      <sheetName val="AEO Table 9 (2019)"/>
+      <sheetName val="AEO Table 16"/>
+      <sheetName val="BGBSC"/>
+      <sheetName val="PAGBSC"/>
+      <sheetName val="SYGBSC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="31">
+          <cell r="A31">
+            <v>1000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="Country Selector"/>
+      <sheetName val="Multipliers and Adjustments"/>
+      <sheetName val="EPA Data"/>
+      <sheetName val="Tech to Policy Mapping"/>
+      <sheetName val="SNAP Adjustment"/>
+      <sheetName val="Cement Data"/>
+      <sheetName val="Data Check"/>
+      <sheetName val="PERAC-cement"/>
+      <sheetName val="PERAC-ngps-mthncptr"/>
+      <sheetName val="PERAC-ngps-mthndstr"/>
+      <sheetName val="PERAC-fgassubstitution"/>
+      <sheetName val="PERAC-fgasdestruction"/>
+      <sheetName val="PERAC-fgasrecovery"/>
+      <sheetName val="PERAC-inspctmaintretrofit"/>
+      <sheetName val="PERAC-coalmining-mthncptr"/>
+      <sheetName val="PERAC-coalmining-mthndstr"/>
+      <sheetName val="PERAC-waste-mthncptr"/>
+      <sheetName val="PERAC-waste-mthndstr"/>
+      <sheetName val="PERAC-cropsrice"/>
+      <sheetName val="PERAC-livestock"/>
+      <sheetName val="PERAC-MCD"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="123">
+          <cell r="A123">
+            <v>1000000000000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,20 +2651,20 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="8" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -712,52 +2672,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -771,7 +2731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>35</v>
       </c>
@@ -792,7 +2752,7 @@
         <v>1.3919999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>36</v>
       </c>
@@ -816,7 +2776,7 @@
         <v>1.2847999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20">
         <v>2013</v>
       </c>
@@ -831,7 +2791,7 @@
         <v>1.3281000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>2014</v>
       </c>
@@ -846,7 +2806,7 @@
         <v>1.3285</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22">
         <v>2015</v>
       </c>
@@ -861,7 +2821,7 @@
         <v>1.1094999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23">
         <v>2016</v>
       </c>
@@ -876,7 +2836,7 @@
         <v>1.1069</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G24">
         <v>2017</v>
       </c>
@@ -891,7 +2851,7 @@
         <v>1.1296999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>2018</v>
       </c>
@@ -906,7 +2866,7 @@
         <v>1.181</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G26">
         <v>2019</v>
       </c>
@@ -921,7 +2881,7 @@
         <v>1.1198999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G27">
         <v>2020</v>
       </c>
@@ -932,7 +2892,7 @@
         <v>1.1422000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G28">
         <v>2021</v>
       </c>
@@ -943,7 +2903,7 @@
         <v>1.1827000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29">
         <v>2022</v>
       </c>
@@ -965,12 +2925,12 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1001,7 +2961,7 @@
       </c>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +2985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1049,7 +3009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +3035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1101,7 +3061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +3087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +3115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +3239,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>D11</f>
         <v>35</v>
@@ -1405,6 +3365,1625 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293040C4-7933-4B72-8968-7BFA5C4D8BE7}">
+  <dimension ref="B1:AG45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2020</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="E9">
+        <v>2022</v>
+      </c>
+      <c r="F9">
+        <v>2023</v>
+      </c>
+      <c r="G9">
+        <v>2024</v>
+      </c>
+      <c r="H9">
+        <v>2025</v>
+      </c>
+      <c r="I9">
+        <v>2026</v>
+      </c>
+      <c r="J9">
+        <v>2027</v>
+      </c>
+      <c r="K9">
+        <v>2028</v>
+      </c>
+      <c r="L9">
+        <v>2029</v>
+      </c>
+      <c r="M9">
+        <v>2030</v>
+      </c>
+      <c r="N9">
+        <v>2031</v>
+      </c>
+      <c r="O9">
+        <v>2032</v>
+      </c>
+      <c r="P9">
+        <v>2033</v>
+      </c>
+      <c r="Q9">
+        <v>2034</v>
+      </c>
+      <c r="R9">
+        <v>2035</v>
+      </c>
+      <c r="S9">
+        <v>2036</v>
+      </c>
+      <c r="T9">
+        <v>2037</v>
+      </c>
+      <c r="U9">
+        <v>2038</v>
+      </c>
+      <c r="V9">
+        <v>2039</v>
+      </c>
+      <c r="W9">
+        <v>2040</v>
+      </c>
+      <c r="X9">
+        <v>2041</v>
+      </c>
+      <c r="Y9">
+        <v>2042</v>
+      </c>
+      <c r="Z9">
+        <v>2043</v>
+      </c>
+      <c r="AA9">
+        <v>2044</v>
+      </c>
+      <c r="AB9">
+        <v>2045</v>
+      </c>
+      <c r="AC9">
+        <v>2046</v>
+      </c>
+      <c r="AD9">
+        <v>2047</v>
+      </c>
+      <c r="AE9">
+        <v>2048</v>
+      </c>
+      <c r="AF9">
+        <v>2049</v>
+      </c>
+      <c r="AG9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="29">
+        <v>1</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1</v>
+      </c>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+      <c r="G10" s="29">
+        <v>1</v>
+      </c>
+      <c r="H10" s="29">
+        <v>1</v>
+      </c>
+      <c r="I10" s="29">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J10" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="K10" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="M10" s="29">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="N10" s="29">
+        <v>0.39</v>
+      </c>
+      <c r="O10" s="29">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q10" s="29">
+        <v>0</v>
+      </c>
+      <c r="R10" s="29">
+        <v>0</v>
+      </c>
+      <c r="S10" s="29">
+        <v>0</v>
+      </c>
+      <c r="T10" s="29">
+        <v>0</v>
+      </c>
+      <c r="U10" s="29">
+        <v>0</v>
+      </c>
+      <c r="V10" s="29">
+        <v>0</v>
+      </c>
+      <c r="W10" s="29">
+        <v>0</v>
+      </c>
+      <c r="X10" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="29">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B11" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="H11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="I11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="J11" s="29">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K11" s="29">
+        <v>0.15</v>
+      </c>
+      <c r="L11" s="29">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="M11" s="29">
+        <v>0</v>
+      </c>
+      <c r="N11" s="29">
+        <v>0</v>
+      </c>
+      <c r="O11" s="29">
+        <v>0</v>
+      </c>
+      <c r="P11" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="29">
+        <v>0</v>
+      </c>
+      <c r="R11" s="29">
+        <v>0</v>
+      </c>
+      <c r="S11" s="29">
+        <v>0</v>
+      </c>
+      <c r="T11" s="29">
+        <v>0</v>
+      </c>
+      <c r="U11" s="29">
+        <v>0</v>
+      </c>
+      <c r="V11" s="29">
+        <v>0</v>
+      </c>
+      <c r="W11" s="29">
+        <v>0</v>
+      </c>
+      <c r="X11" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="29">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2020</v>
+      </c>
+      <c r="D14">
+        <v>2021</v>
+      </c>
+      <c r="E14">
+        <v>2022</v>
+      </c>
+      <c r="F14">
+        <v>2023</v>
+      </c>
+      <c r="G14">
+        <v>2024</v>
+      </c>
+      <c r="H14">
+        <v>2025</v>
+      </c>
+      <c r="I14">
+        <v>2026</v>
+      </c>
+      <c r="J14">
+        <v>2027</v>
+      </c>
+      <c r="K14">
+        <v>2028</v>
+      </c>
+      <c r="L14">
+        <v>2029</v>
+      </c>
+      <c r="M14">
+        <v>2030</v>
+      </c>
+      <c r="N14">
+        <v>2031</v>
+      </c>
+      <c r="O14">
+        <v>2032</v>
+      </c>
+      <c r="P14">
+        <v>2033</v>
+      </c>
+      <c r="Q14">
+        <v>2034</v>
+      </c>
+      <c r="R14">
+        <v>2035</v>
+      </c>
+      <c r="S14">
+        <v>2036</v>
+      </c>
+      <c r="T14">
+        <v>2037</v>
+      </c>
+      <c r="U14">
+        <v>2038</v>
+      </c>
+      <c r="V14">
+        <v>2039</v>
+      </c>
+      <c r="W14">
+        <v>2040</v>
+      </c>
+      <c r="X14">
+        <v>2041</v>
+      </c>
+      <c r="Y14">
+        <v>2042</v>
+      </c>
+      <c r="Z14">
+        <v>2043</v>
+      </c>
+      <c r="AA14">
+        <v>2044</v>
+      </c>
+      <c r="AB14">
+        <v>2045</v>
+      </c>
+      <c r="AC14">
+        <v>2046</v>
+      </c>
+      <c r="AD14">
+        <v>2047</v>
+      </c>
+      <c r="AE14">
+        <v>2048</v>
+      </c>
+      <c r="AF14">
+        <v>2049</v>
+      </c>
+      <c r="AG14">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="29">
+        <f>1-C10</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="29">
+        <f t="shared" ref="D15:AG15" si="0">1-D10</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="L15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="M15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="N15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="O15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+      <c r="Q15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AB15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AF15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AG15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="29">
+        <f t="shared" ref="C16:AG16" si="1">1-C11</f>
+        <v>0.7</v>
+      </c>
+      <c r="D16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="F16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="H16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="I16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="J16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="L16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="M16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="V16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="W16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Z16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AE16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AG16" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <v>2022</v>
+      </c>
+      <c r="D36">
+        <v>2023</v>
+      </c>
+      <c r="E36">
+        <v>2024</v>
+      </c>
+      <c r="F36">
+        <v>2025</v>
+      </c>
+      <c r="G36">
+        <v>2026</v>
+      </c>
+      <c r="H36">
+        <v>2027</v>
+      </c>
+      <c r="I36">
+        <v>2028</v>
+      </c>
+      <c r="J36">
+        <v>2029</v>
+      </c>
+      <c r="K36">
+        <v>2030</v>
+      </c>
+      <c r="L36">
+        <v>2031</v>
+      </c>
+      <c r="M36">
+        <v>2032</v>
+      </c>
+      <c r="N36">
+        <v>2033</v>
+      </c>
+      <c r="O36">
+        <v>2034</v>
+      </c>
+      <c r="P36">
+        <v>2035</v>
+      </c>
+      <c r="Q36">
+        <v>2036</v>
+      </c>
+      <c r="R36">
+        <v>2037</v>
+      </c>
+      <c r="S36">
+        <v>2038</v>
+      </c>
+      <c r="T36">
+        <v>2039</v>
+      </c>
+      <c r="U36">
+        <v>2040</v>
+      </c>
+      <c r="V36">
+        <v>2041</v>
+      </c>
+      <c r="W36">
+        <v>2042</v>
+      </c>
+      <c r="X36">
+        <v>2043</v>
+      </c>
+      <c r="Y36">
+        <v>2044</v>
+      </c>
+      <c r="Z36">
+        <v>2045</v>
+      </c>
+      <c r="AA36">
+        <v>2046</v>
+      </c>
+      <c r="AB36">
+        <v>2047</v>
+      </c>
+      <c r="AC36">
+        <v>2048</v>
+      </c>
+      <c r="AD36">
+        <v>2049</v>
+      </c>
+      <c r="AE36">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="30">
+        <v>821630000000000</v>
+      </c>
+      <c r="D37" s="30">
+        <v>835002000000000</v>
+      </c>
+      <c r="E37" s="30">
+        <v>842990000000000</v>
+      </c>
+      <c r="F37" s="30">
+        <v>847879000000000</v>
+      </c>
+      <c r="G37" s="30">
+        <v>837634000000000</v>
+      </c>
+      <c r="H37" s="30">
+        <v>823562000000000</v>
+      </c>
+      <c r="I37" s="30">
+        <v>811581000000000</v>
+      </c>
+      <c r="J37" s="30">
+        <v>795773000000000</v>
+      </c>
+      <c r="K37" s="30">
+        <v>776260000000000</v>
+      </c>
+      <c r="L37" s="30">
+        <v>755704000000000</v>
+      </c>
+      <c r="M37" s="30">
+        <v>734255000000000</v>
+      </c>
+      <c r="N37" s="30">
+        <v>712009000000000</v>
+      </c>
+      <c r="O37" s="30">
+        <v>686996000000000</v>
+      </c>
+      <c r="P37" s="30">
+        <v>664207000000000</v>
+      </c>
+      <c r="Q37" s="30">
+        <v>642324000000000</v>
+      </c>
+      <c r="R37" s="30">
+        <v>620364000000000</v>
+      </c>
+      <c r="S37" s="30">
+        <v>596761000000000</v>
+      </c>
+      <c r="T37" s="30">
+        <v>578179000000000</v>
+      </c>
+      <c r="U37" s="30">
+        <v>560791000000000</v>
+      </c>
+      <c r="V37" s="30">
+        <v>540441000000000</v>
+      </c>
+      <c r="W37" s="30">
+        <v>524324000000000</v>
+      </c>
+      <c r="X37" s="30">
+        <v>509657000000000</v>
+      </c>
+      <c r="Y37" s="30">
+        <v>494492000000000</v>
+      </c>
+      <c r="Z37" s="30">
+        <v>481727000000000</v>
+      </c>
+      <c r="AA37" s="30">
+        <v>468499000000000</v>
+      </c>
+      <c r="AB37" s="30">
+        <v>457626000000000</v>
+      </c>
+      <c r="AC37" s="30">
+        <v>446360000000000</v>
+      </c>
+      <c r="AD37" s="30">
+        <v>437154000000000</v>
+      </c>
+      <c r="AE37" s="30">
+        <v>428031000000000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="30">
+        <v>638953000000000</v>
+      </c>
+      <c r="D38" s="30">
+        <v>608440000000000</v>
+      </c>
+      <c r="E38" s="30">
+        <v>534928000000000</v>
+      </c>
+      <c r="F38" s="30">
+        <v>517601000000000</v>
+      </c>
+      <c r="G38" s="30">
+        <v>456956000000000</v>
+      </c>
+      <c r="H38" s="30">
+        <v>385949000000000</v>
+      </c>
+      <c r="I38" s="30">
+        <v>305127000000000</v>
+      </c>
+      <c r="J38" s="30">
+        <v>215547000000000</v>
+      </c>
+      <c r="K38" s="30">
+        <v>112200000000000</v>
+      </c>
+      <c r="L38" s="30">
+        <v>79291900000000</v>
+      </c>
+      <c r="M38" s="30">
+        <v>66275700000000</v>
+      </c>
+      <c r="N38" s="30">
+        <v>52177600000000</v>
+      </c>
+      <c r="O38" s="30">
+        <v>42506000000000</v>
+      </c>
+      <c r="P38" s="30">
+        <v>34311300000000</v>
+      </c>
+      <c r="Q38" s="30">
+        <v>27234100000000</v>
+      </c>
+      <c r="R38" s="30">
+        <v>24714500000000</v>
+      </c>
+      <c r="S38" s="30">
+        <v>21579400000000</v>
+      </c>
+      <c r="T38" s="30">
+        <v>20412300000000</v>
+      </c>
+      <c r="U38" s="30">
+        <v>16762300000000</v>
+      </c>
+      <c r="V38" s="30">
+        <v>23135800000000</v>
+      </c>
+      <c r="W38" s="30">
+        <v>24620100000000</v>
+      </c>
+      <c r="X38" s="30">
+        <v>25877200000000</v>
+      </c>
+      <c r="Y38" s="30">
+        <v>26128200000000</v>
+      </c>
+      <c r="Z38" s="30">
+        <v>22537400000000</v>
+      </c>
+      <c r="AA38" s="30">
+        <v>30070400000000</v>
+      </c>
+      <c r="AB38" s="30">
+        <v>26010400000000</v>
+      </c>
+      <c r="AC38" s="30">
+        <v>26908800000000</v>
+      </c>
+      <c r="AD38" s="30">
+        <v>25621600000000</v>
+      </c>
+      <c r="AE38" s="30">
+        <v>20709600000000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="30">
+        <v>322904000000000</v>
+      </c>
+      <c r="D39" s="30">
+        <v>317119000000000</v>
+      </c>
+      <c r="E39" s="30">
+        <v>306079000000000</v>
+      </c>
+      <c r="F39" s="30">
+        <v>304412000000000</v>
+      </c>
+      <c r="G39" s="30">
+        <v>300384000000000</v>
+      </c>
+      <c r="H39" s="30">
+        <v>295654000000000</v>
+      </c>
+      <c r="I39" s="30">
+        <v>295022000000000</v>
+      </c>
+      <c r="J39" s="30">
+        <v>293093000000000</v>
+      </c>
+      <c r="K39" s="30">
+        <v>290114000000000</v>
+      </c>
+      <c r="L39" s="30">
+        <v>286926000000000</v>
+      </c>
+      <c r="M39" s="30">
+        <v>285577000000000</v>
+      </c>
+      <c r="N39" s="30">
+        <v>283934000000000</v>
+      </c>
+      <c r="O39" s="30">
+        <v>283202000000000</v>
+      </c>
+      <c r="P39" s="30">
+        <v>279505000000000</v>
+      </c>
+      <c r="Q39" s="30">
+        <v>276457000000000</v>
+      </c>
+      <c r="R39" s="30">
+        <v>273860000000000</v>
+      </c>
+      <c r="S39" s="30">
+        <v>271912000000000</v>
+      </c>
+      <c r="T39" s="30">
+        <v>269450000000000</v>
+      </c>
+      <c r="U39" s="30">
+        <v>266965000000000</v>
+      </c>
+      <c r="V39" s="30">
+        <v>264703000000000</v>
+      </c>
+      <c r="W39" s="30">
+        <v>262338000000000</v>
+      </c>
+      <c r="X39" s="30">
+        <v>259890000000000</v>
+      </c>
+      <c r="Y39" s="30">
+        <v>257529000000000</v>
+      </c>
+      <c r="Z39" s="30">
+        <v>255367000000000</v>
+      </c>
+      <c r="AA39" s="30">
+        <v>253008000000000</v>
+      </c>
+      <c r="AB39" s="30">
+        <v>250560000000000</v>
+      </c>
+      <c r="AC39" s="30">
+        <v>247809000000000</v>
+      </c>
+      <c r="AD39" s="30">
+        <v>245248000000000</v>
+      </c>
+      <c r="AE39" s="30">
+        <v>242653000000000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="30">
+        <v>125080000000000</v>
+      </c>
+      <c r="D40" s="30">
+        <v>122328000000000</v>
+      </c>
+      <c r="E40" s="30">
+        <v>117531000000000</v>
+      </c>
+      <c r="F40" s="30">
+        <v>116908000000000</v>
+      </c>
+      <c r="G40" s="30">
+        <v>114827000000000</v>
+      </c>
+      <c r="H40" s="30">
+        <v>112418000000000</v>
+      </c>
+      <c r="I40" s="30">
+        <v>111972000000000</v>
+      </c>
+      <c r="J40" s="30">
+        <v>110632000000000</v>
+      </c>
+      <c r="K40" s="30">
+        <v>109170000000000</v>
+      </c>
+      <c r="L40" s="30">
+        <v>107343000000000</v>
+      </c>
+      <c r="M40" s="30">
+        <v>106214000000000</v>
+      </c>
+      <c r="N40" s="30">
+        <v>105017000000000</v>
+      </c>
+      <c r="O40" s="30">
+        <v>104194000000000</v>
+      </c>
+      <c r="P40" s="30">
+        <v>102314000000000</v>
+      </c>
+      <c r="Q40" s="30">
+        <v>100439000000000</v>
+      </c>
+      <c r="R40" s="30">
+        <v>98823900000000</v>
+      </c>
+      <c r="S40" s="30">
+        <v>97504000000000</v>
+      </c>
+      <c r="T40" s="30">
+        <v>96036600000000</v>
+      </c>
+      <c r="U40" s="30">
+        <v>94621000000000</v>
+      </c>
+      <c r="V40" s="30">
+        <v>93200000000000</v>
+      </c>
+      <c r="W40" s="30">
+        <v>91887500000000</v>
+      </c>
+      <c r="X40" s="30">
+        <v>90459500000000</v>
+      </c>
+      <c r="Y40" s="30">
+        <v>89109500000000</v>
+      </c>
+      <c r="Z40" s="30">
+        <v>87951700000000</v>
+      </c>
+      <c r="AA40" s="30">
+        <v>86709300000000</v>
+      </c>
+      <c r="AB40" s="30">
+        <v>85534300000000</v>
+      </c>
+      <c r="AC40" s="30">
+        <v>84269200000000</v>
+      </c>
+      <c r="AD40" s="30">
+        <v>83411800000000</v>
+      </c>
+      <c r="AE40" s="30">
+        <v>82481200000000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="30">
+        <v>1451180000000000</v>
+      </c>
+      <c r="D41" s="30">
+        <v>1462180000000000</v>
+      </c>
+      <c r="E41" s="30">
+        <v>1463280000000000</v>
+      </c>
+      <c r="F41" s="30">
+        <v>1466410000000000</v>
+      </c>
+      <c r="G41" s="30">
+        <v>1471300000000000</v>
+      </c>
+      <c r="H41" s="30">
+        <v>1462350000000000</v>
+      </c>
+      <c r="I41" s="30">
+        <v>1451050000000000</v>
+      </c>
+      <c r="J41" s="30">
+        <v>1440130000000000</v>
+      </c>
+      <c r="K41" s="30">
+        <v>1427490000000000</v>
+      </c>
+      <c r="L41" s="30">
+        <v>1414920000000000</v>
+      </c>
+      <c r="M41" s="30">
+        <v>1404060000000000</v>
+      </c>
+      <c r="N41" s="30">
+        <v>1390550000000000</v>
+      </c>
+      <c r="O41" s="30">
+        <v>1378680000000000</v>
+      </c>
+      <c r="P41" s="30">
+        <v>1366830000000000</v>
+      </c>
+      <c r="Q41" s="30">
+        <v>1360360000000000</v>
+      </c>
+      <c r="R41" s="30">
+        <v>1350520000000000</v>
+      </c>
+      <c r="S41" s="30">
+        <v>1341760000000000</v>
+      </c>
+      <c r="T41" s="30">
+        <v>1332110000000000</v>
+      </c>
+      <c r="U41" s="30">
+        <v>1321190000000000</v>
+      </c>
+      <c r="V41" s="30">
+        <v>1310080000000000</v>
+      </c>
+      <c r="W41" s="30">
+        <v>1302190000000000</v>
+      </c>
+      <c r="X41" s="30">
+        <v>1292620000000000</v>
+      </c>
+      <c r="Y41" s="30">
+        <v>1285730000000000</v>
+      </c>
+      <c r="Z41" s="30">
+        <v>1280150000000000</v>
+      </c>
+      <c r="AA41" s="30">
+        <v>1275200000000000</v>
+      </c>
+      <c r="AB41" s="30">
+        <v>1266610000000000</v>
+      </c>
+      <c r="AC41" s="30">
+        <v>1261140000000000</v>
+      </c>
+      <c r="AD41" s="30">
+        <v>1254830000000000</v>
+      </c>
+      <c r="AE41" s="30">
+        <v>1246830000000000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="30">
+        <v>123893000000000</v>
+      </c>
+      <c r="D42" s="30">
+        <v>118154000000000</v>
+      </c>
+      <c r="E42" s="30">
+        <v>115601000000000</v>
+      </c>
+      <c r="F42" s="30">
+        <v>113870000000000</v>
+      </c>
+      <c r="G42" s="30">
+        <v>113982000000000</v>
+      </c>
+      <c r="H42" s="30">
+        <v>113273000000000</v>
+      </c>
+      <c r="I42" s="30">
+        <v>111739000000000</v>
+      </c>
+      <c r="J42" s="30">
+        <v>110915000000000</v>
+      </c>
+      <c r="K42" s="30">
+        <v>108839000000000</v>
+      </c>
+      <c r="L42" s="30">
+        <v>107407000000000</v>
+      </c>
+      <c r="M42" s="30">
+        <v>105960000000000</v>
+      </c>
+      <c r="N42" s="30">
+        <v>104827000000000</v>
+      </c>
+      <c r="O42" s="30">
+        <v>103488000000000</v>
+      </c>
+      <c r="P42" s="30">
+        <v>102109000000000</v>
+      </c>
+      <c r="Q42" s="30">
+        <v>102358000000000</v>
+      </c>
+      <c r="R42" s="30">
+        <v>102641000000000</v>
+      </c>
+      <c r="S42" s="30">
+        <v>103089000000000</v>
+      </c>
+      <c r="T42" s="30">
+        <v>103361000000000</v>
+      </c>
+      <c r="U42" s="30">
+        <v>102565000000000</v>
+      </c>
+      <c r="V42" s="30">
+        <v>103020000000000</v>
+      </c>
+      <c r="W42" s="30">
+        <v>103716000000000</v>
+      </c>
+      <c r="X42" s="30">
+        <v>103344000000000</v>
+      </c>
+      <c r="Y42" s="30">
+        <v>103838000000000</v>
+      </c>
+      <c r="Z42" s="30">
+        <v>104006000000000</v>
+      </c>
+      <c r="AA42" s="30">
+        <v>104613000000000</v>
+      </c>
+      <c r="AB42" s="30">
+        <v>105638000000000</v>
+      </c>
+      <c r="AC42" s="30">
+        <v>106471000000000</v>
+      </c>
+      <c r="AD42" s="30">
+        <v>107252000000000</v>
+      </c>
+      <c r="AE42" s="30">
+        <v>108054000000000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="30">
+        <v>-239792000000000</v>
+      </c>
+      <c r="D43" s="30">
+        <v>-234893000000000</v>
+      </c>
+      <c r="E43" s="30">
+        <v>-234893000000000</v>
+      </c>
+      <c r="F43" s="30">
+        <v>-235882000000000</v>
+      </c>
+      <c r="G43" s="30">
+        <v>-231942000000000</v>
+      </c>
+      <c r="H43" s="30">
+        <v>-231942000000000</v>
+      </c>
+      <c r="I43" s="30">
+        <v>-231947000000000</v>
+      </c>
+      <c r="J43" s="30">
+        <v>-232937000000000</v>
+      </c>
+      <c r="K43" s="30">
+        <v>-234893000000000</v>
+      </c>
+      <c r="L43" s="30">
+        <v>-232939000000000</v>
+      </c>
+      <c r="M43" s="30">
+        <v>-232939000000000</v>
+      </c>
+      <c r="N43" s="30">
+        <v>-228035000000000</v>
+      </c>
+      <c r="O43" s="30">
+        <v>-227059000000000</v>
+      </c>
+      <c r="P43" s="30">
+        <v>-226081000000000</v>
+      </c>
+      <c r="Q43" s="30">
+        <v>-224117000000000</v>
+      </c>
+      <c r="R43" s="30">
+        <v>-222158000000000</v>
+      </c>
+      <c r="S43" s="30">
+        <v>-220196000000000</v>
+      </c>
+      <c r="T43" s="30">
+        <v>-219234000000000</v>
+      </c>
+      <c r="U43" s="30">
+        <v>-217272000000000</v>
+      </c>
+      <c r="V43" s="30">
+        <v>-215311000000000</v>
+      </c>
+      <c r="W43" s="30">
+        <v>-213349000000000</v>
+      </c>
+      <c r="X43" s="30">
+        <v>-211390000000000</v>
+      </c>
+      <c r="Y43" s="30">
+        <v>-210425000000000</v>
+      </c>
+      <c r="Z43" s="30">
+        <v>-208464000000000</v>
+      </c>
+      <c r="AA43" s="30">
+        <v>-206502000000000</v>
+      </c>
+      <c r="AB43" s="30">
+        <v>-204540000000000</v>
+      </c>
+      <c r="AC43" s="30">
+        <v>-202579000000000</v>
+      </c>
+      <c r="AD43" s="30">
+        <v>-201617000000000</v>
+      </c>
+      <c r="AE43" s="30">
+        <v>-199658000000000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44">
+        <v>0</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
+      </c>
+      <c r="AC44">
+        <v>0</v>
+      </c>
+      <c r="AD44">
+        <v>0</v>
+      </c>
+      <c r="AE44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="30">
+        <v>62635600000000</v>
+      </c>
+      <c r="D45" s="30">
+        <v>59439900000000</v>
+      </c>
+      <c r="E45" s="30">
+        <v>59843900000000</v>
+      </c>
+      <c r="F45" s="30">
+        <v>60321800000000</v>
+      </c>
+      <c r="G45" s="30">
+        <v>62896300000000</v>
+      </c>
+      <c r="H45" s="30">
+        <v>64734400000000</v>
+      </c>
+      <c r="I45" s="30">
+        <v>65779500000000</v>
+      </c>
+      <c r="J45" s="30">
+        <v>67744100000000</v>
+      </c>
+      <c r="K45" s="30">
+        <v>69724900000000</v>
+      </c>
+      <c r="L45" s="30">
+        <v>70274200000000</v>
+      </c>
+      <c r="M45" s="30">
+        <v>70571200000000</v>
+      </c>
+      <c r="N45" s="30">
+        <v>71033100000000</v>
+      </c>
+      <c r="O45" s="30">
+        <v>71586700000000</v>
+      </c>
+      <c r="P45" s="30">
+        <v>72248100000000</v>
+      </c>
+      <c r="Q45" s="30">
+        <v>73544100000000</v>
+      </c>
+      <c r="R45" s="30">
+        <v>74732400000000</v>
+      </c>
+      <c r="S45" s="30">
+        <v>76047000000000</v>
+      </c>
+      <c r="T45" s="30">
+        <v>77306100000000</v>
+      </c>
+      <c r="U45" s="30">
+        <v>78819700000000</v>
+      </c>
+      <c r="V45" s="30">
+        <v>79834200000000</v>
+      </c>
+      <c r="W45" s="30">
+        <v>81102500000000</v>
+      </c>
+      <c r="X45" s="30">
+        <v>81312900000000</v>
+      </c>
+      <c r="Y45" s="30">
+        <v>82474700000000</v>
+      </c>
+      <c r="Z45" s="30">
+        <v>83583400000000</v>
+      </c>
+      <c r="AA45" s="30">
+        <v>84752000000000</v>
+      </c>
+      <c r="AB45" s="30">
+        <v>86210800000000</v>
+      </c>
+      <c r="AC45" s="30">
+        <v>87529800000000</v>
+      </c>
+      <c r="AD45" s="30">
+        <v>88856100000000</v>
+      </c>
+      <c r="AE45" s="30">
+        <v>90267000000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" display="Free allowances to other industries" xr:uid="{3CA7A010-3535-4F25-9BD0-52037EDB8016}"/>
+    <hyperlink ref="B10" r:id="rId2" display="Free allowances to high-leak-risk industries" xr:uid="{7A0B70FD-C22B-4CF8-B50A-84293460D74A}"/>
+    <hyperlink ref="B16" r:id="rId3" display="Free allowances to other industries" xr:uid="{4BAF2E08-9D96-4FB3-BE3D-111F36D33C47}"/>
+    <hyperlink ref="B15" r:id="rId4" display="Free allowances to high-leak-risk industries" xr:uid="{931557CF-2723-4493-B204-FD510C7CF3BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A588720-4507-45D9-BCC3-2B2208374E22}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
@@ -1412,15 +4991,15 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1515,7 +5094,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1640,7 +5219,7 @@
         <v>90.517287831162989</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1765,7 +5344,7 @@
         <v>90.517287831162989</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1955,7 +5534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2080,132 +5659,132 @@
         <v>90.517287831162989</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="24">
-        <f>B6*0.75*0.6</f>
-        <v>15.840525370453523</v>
+        <f>B6*(('Allowance Schedule'!C45/'Allowance Schedule'!C42)*'Allowance Schedule'!D15+(1-'Allowance Schedule'!C45/'Allowance Schedule'!C42))</f>
+        <v>17.404792824417839</v>
       </c>
       <c r="C7" s="24">
-        <f t="shared" ref="C7:AE7" si="3">C6*0.75*0.6</f>
-        <v>15.840525370453523</v>
+        <f>C6*(('Allowance Schedule'!C45/'Allowance Schedule'!C42)*'Allowance Schedule'!D15+(1-'Allowance Schedule'!C45/'Allowance Schedule'!C42))</f>
+        <v>17.404792824417839</v>
       </c>
       <c r="D7" s="24">
-        <f t="shared" si="3"/>
-        <v>15.840525370453523</v>
+        <f>D6*(('Allowance Schedule'!D45/'Allowance Schedule'!D42)*'Allowance Schedule'!E15+(1-'Allowance Schedule'!D45/'Allowance Schedule'!D42))</f>
+        <v>17.492466341541927</v>
       </c>
       <c r="E7" s="24">
-        <f t="shared" si="3"/>
-        <v>15.840525370453523</v>
+        <f>E6*(('Allowance Schedule'!E45/'Allowance Schedule'!E42)*'Allowance Schedule'!F15+(1-'Allowance Schedule'!E45/'Allowance Schedule'!E42))</f>
+        <v>16.978356725728325</v>
       </c>
       <c r="F7" s="24">
-        <f t="shared" si="3"/>
-        <v>15.840525370453523</v>
+        <f>F6*(('Allowance Schedule'!F45/'Allowance Schedule'!F42)*'Allowance Schedule'!G15+(1-'Allowance Schedule'!F45/'Allowance Schedule'!F42))</f>
+        <v>16.55360636675584</v>
       </c>
       <c r="G7" s="24">
-        <f t="shared" si="3"/>
-        <v>17.198284687920971</v>
+        <f>G6*(('Allowance Schedule'!G45/'Allowance Schedule'!G42)*'Allowance Schedule'!H15+(1-'Allowance Schedule'!G45/'Allowance Schedule'!G42))</f>
+        <v>17.129145383222777</v>
       </c>
       <c r="H7" s="24">
-        <f t="shared" si="3"/>
-        <v>18.556044005388411</v>
+        <f>H6*(('Allowance Schedule'!H45/'Allowance Schedule'!H42)*'Allowance Schedule'!I15+(1-'Allowance Schedule'!H45/'Allowance Schedule'!H42))</f>
+        <v>18.25902920744095</v>
       </c>
       <c r="I7" s="24">
-        <f t="shared" si="3"/>
-        <v>19.913803322855859</v>
+        <f>I6*(('Allowance Schedule'!I45/'Allowance Schedule'!I42)*'Allowance Schedule'!J15+(1-'Allowance Schedule'!I45/'Allowance Schedule'!I42))</f>
+        <v>19.504270270711885</v>
       </c>
       <c r="J7" s="24">
-        <f t="shared" si="3"/>
-        <v>21.271562640323303</v>
+        <f>J6*(('Allowance Schedule'!J45/'Allowance Schedule'!J42)*'Allowance Schedule'!K15+(1-'Allowance Schedule'!J45/'Allowance Schedule'!J42))</f>
+        <v>21.285865357463241</v>
       </c>
       <c r="K7" s="24">
-        <f t="shared" si="3"/>
-        <v>22.629321957790751</v>
+        <f>K6*(('Allowance Schedule'!K45/'Allowance Schedule'!K42)*'Allowance Schedule'!L15+(1-'Allowance Schedule'!K45/'Allowance Schedule'!K42))</f>
+        <v>25.320512854737427</v>
       </c>
       <c r="L7" s="24">
-        <f t="shared" si="3"/>
-        <v>23.534494836102382</v>
+        <f>L6*(('Allowance Schedule'!L45/'Allowance Schedule'!L42)*'Allowance Schedule'!M15+(1-'Allowance Schedule'!L45/'Allowance Schedule'!L42))</f>
+        <v>34.676564043528451</v>
       </c>
       <c r="M7" s="24">
-        <f t="shared" si="3"/>
-        <v>24.439667714414011</v>
+        <f>M6*(('Allowance Schedule'!M45/'Allowance Schedule'!M42)*'Allowance Schedule'!N15+(1-'Allowance Schedule'!M45/'Allowance Schedule'!M42))</f>
+        <v>40.203428684165964</v>
       </c>
       <c r="N7" s="24">
-        <f t="shared" si="3"/>
-        <v>25.344840592725642</v>
+        <f>N6*(('Allowance Schedule'!N45/'Allowance Schedule'!N42)*'Allowance Schedule'!O15+(1-'Allowance Schedule'!N45/'Allowance Schedule'!N42))</f>
+        <v>46.208157075568081</v>
       </c>
       <c r="O7" s="24">
-        <f t="shared" si="3"/>
-        <v>26.250013471037267</v>
+        <f>O6*(('Allowance Schedule'!O45/'Allowance Schedule'!O42)*'Allowance Schedule'!P15+(1-'Allowance Schedule'!O45/'Allowance Schedule'!O42))</f>
+        <v>52.684157402728609</v>
       </c>
       <c r="P7" s="24">
-        <f t="shared" si="3"/>
-        <v>27.155186349348895</v>
+        <f>P6*(('Allowance Schedule'!P45/'Allowance Schedule'!P42)*'Allowance Schedule'!Q15+(1-'Allowance Schedule'!P45/'Allowance Schedule'!P42))</f>
+        <v>60.344858554108662</v>
       </c>
       <c r="Q7" s="24">
-        <f t="shared" si="3"/>
-        <v>28.060359227660527</v>
+        <f>Q6*(('Allowance Schedule'!Q45/'Allowance Schedule'!Q42)*'Allowance Schedule'!R15+(1-'Allowance Schedule'!Q45/'Allowance Schedule'!Q42))</f>
+        <v>62.356353839245621</v>
       </c>
       <c r="R7" s="24">
-        <f t="shared" si="3"/>
-        <v>28.965532105972155</v>
+        <f>R6*(('Allowance Schedule'!R45/'Allowance Schedule'!R42)*'Allowance Schedule'!S15+(1-'Allowance Schedule'!R45/'Allowance Schedule'!R42))</f>
+        <v>64.367849124382573</v>
       </c>
       <c r="S7" s="24">
-        <f t="shared" si="3"/>
-        <v>29.870704984283787</v>
+        <f>S6*(('Allowance Schedule'!S45/'Allowance Schedule'!S42)*'Allowance Schedule'!T15+(1-'Allowance Schedule'!S45/'Allowance Schedule'!S42))</f>
+        <v>66.379344409519533</v>
       </c>
       <c r="T7" s="24">
-        <f t="shared" si="3"/>
-        <v>30.775877862595415</v>
+        <f>T6*(('Allowance Schedule'!T45/'Allowance Schedule'!T42)*'Allowance Schedule'!U15+(1-'Allowance Schedule'!T45/'Allowance Schedule'!T42))</f>
+        <v>68.390839694656478</v>
       </c>
       <c r="U7" s="24">
-        <f t="shared" si="3"/>
-        <v>31.681050740907047</v>
+        <f>U6*(('Allowance Schedule'!U45/'Allowance Schedule'!U42)*'Allowance Schedule'!V15+(1-'Allowance Schedule'!U45/'Allowance Schedule'!U42))</f>
+        <v>70.402334979793437</v>
       </c>
       <c r="V7" s="24">
-        <f t="shared" si="3"/>
-        <v>32.586223619218678</v>
+        <f>V6*(('Allowance Schedule'!V45/'Allowance Schedule'!V42)*'Allowance Schedule'!W15+(1-'Allowance Schedule'!V45/'Allowance Schedule'!V42))</f>
+        <v>72.413830264930397</v>
       </c>
       <c r="W7" s="24">
-        <f t="shared" si="3"/>
-        <v>33.49139649753031</v>
+        <f>W6*(('Allowance Schedule'!W45/'Allowance Schedule'!W42)*'Allowance Schedule'!X15+(1-'Allowance Schedule'!W45/'Allowance Schedule'!W42))</f>
+        <v>74.425325550067356</v>
       </c>
       <c r="X7" s="24">
-        <f t="shared" si="3"/>
-        <v>34.396569375841942</v>
+        <f>X6*(('Allowance Schedule'!X45/'Allowance Schedule'!X42)*'Allowance Schedule'!Y15+(1-'Allowance Schedule'!X45/'Allowance Schedule'!X42))</f>
+        <v>76.436820835204315</v>
       </c>
       <c r="Y7" s="24">
-        <f t="shared" si="3"/>
-        <v>35.301742254153567</v>
+        <f>Y6*(('Allowance Schedule'!Y45/'Allowance Schedule'!Y42)*'Allowance Schedule'!Z15+(1-'Allowance Schedule'!Y45/'Allowance Schedule'!Y42))</f>
+        <v>78.448316120341261</v>
       </c>
       <c r="Z7" s="24">
-        <f t="shared" si="3"/>
-        <v>36.206915132465198</v>
+        <f>Z6*(('Allowance Schedule'!Z45/'Allowance Schedule'!Z42)*'Allowance Schedule'!AA15+(1-'Allowance Schedule'!Z45/'Allowance Schedule'!Z42))</f>
+        <v>80.45981140547822</v>
       </c>
       <c r="AA7" s="24">
-        <f t="shared" si="3"/>
-        <v>37.112088010776823</v>
+        <f>AA6*(('Allowance Schedule'!AA45/'Allowance Schedule'!AA42)*'Allowance Schedule'!AB15+(1-'Allowance Schedule'!AA45/'Allowance Schedule'!AA42))</f>
+        <v>82.471306690615165</v>
       </c>
       <c r="AB7" s="24">
-        <f t="shared" si="3"/>
-        <v>38.017260889088462</v>
+        <f>AB6*(('Allowance Schedule'!AB45/'Allowance Schedule'!AB42)*'Allowance Schedule'!AC15+(1-'Allowance Schedule'!AB45/'Allowance Schedule'!AB42))</f>
+        <v>84.482801975752139</v>
       </c>
       <c r="AC7" s="24">
-        <f t="shared" si="3"/>
-        <v>38.922433767400086</v>
+        <f>AC6*(('Allowance Schedule'!AC45/'Allowance Schedule'!AC42)*'Allowance Schedule'!AD15+(1-'Allowance Schedule'!AC45/'Allowance Schedule'!AC42))</f>
+        <v>86.494297260889084</v>
       </c>
       <c r="AD7" s="24">
-        <f t="shared" si="3"/>
-        <v>39.827606645711718</v>
+        <f>AD6*(('Allowance Schedule'!AD45/'Allowance Schedule'!AD42)*'Allowance Schedule'!AE15+(1-'Allowance Schedule'!AD45/'Allowance Schedule'!AD42))</f>
+        <v>88.505792546026044</v>
       </c>
       <c r="AE7" s="24">
-        <f t="shared" si="3"/>
-        <v>40.732779524023343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+        <f>AE6*(('Allowance Schedule'!AE45/'Allowance Schedule'!AE42)*'Allowance Schedule'!AF15+(1-'Allowance Schedule'!AE45/'Allowance Schedule'!AE42))</f>
+        <v>90.517287831162989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2300,7 +5879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2402,6 +5981,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -2630,27 +6229,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3810981-6F61-4C76-A985-60AA740A519D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2667,23 +6265,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7AEB696-AA90-45CB-B453-739D51A4BE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187D143-7832-42EF-BDC9-4813FDEF40F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>